<commit_message>
Addition of SciTech presentation materials
Added various files used for the presentation at the AIAA SciTech conference in San Diego, CA.
</commit_message>
<xml_diff>
--- a/cs1-2/Submissions/Case1/iea37-cs1-aepranks.xlsx
+++ b/cs1-2/Submissions/Case1/iea37-cs1-aepranks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbaker/Documents/GitHub/iea37-casestudies-extrafiles/Submissions/Case1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbaker/Documents/GitHub/iea37-casestudies-extrafiles/cs1-2/Submissions/Case1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
   <si>
     <t>AEP</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>Wall Time  (s)</t>
+  </si>
+  <si>
+    <t>Salhi</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>Phil</t>
   </si>
 </sst>
 </file>
@@ -238,7 +247,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -255,6 +264,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -538,25 +548,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L39"/>
+  <dimension ref="A2:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="178" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="178" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="4.5" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="4.5" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -570,25 +581,28 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -598,14 +612,15 @@
       <c r="D3" s="1">
         <v>366941.57115999999</v>
       </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -615,26 +630,27 @@
       <c r="D4" s="1">
         <v>411182.219979972</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="10"/>
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2889</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>50</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -644,26 +660,27 @@
       <c r="D5" s="1">
         <v>409689.44173999998</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="10"/>
+      <c r="F5">
         <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1000</v>
       </c>
       <c r="G5">
         <v>1000</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="J5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -673,26 +690,27 @@
       <c r="D6" s="1">
         <v>402318.75670000003</v>
       </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
+      <c r="E6" s="10"/>
       <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
         <v>100</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>150</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -702,23 +720,24 @@
       <c r="D7" s="1">
         <v>418924.40636295598</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="10"/>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>696</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>615</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -728,24 +747,25 @@
       <c r="D8" s="1">
         <v>414141.29376099998</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
+      <c r="E8" s="10"/>
       <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8">
         <v>38100</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" t="s">
+      <c r="I8" s="2"/>
+      <c r="J8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -755,20 +775,21 @@
       <c r="D9" s="1">
         <v>388758.35729000001</v>
       </c>
-      <c r="E9">
-        <v>9</v>
-      </c>
+      <c r="E9" s="10"/>
       <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
         <v>6000</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>300</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -778,23 +799,24 @@
       <c r="D10" s="1">
         <v>392587.85803100001</v>
       </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
+      <c r="E10" s="10"/>
       <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
         <v>37500</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>25</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -804,23 +826,24 @@
       <c r="D11" s="1">
         <v>412251.19453009701</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="10"/>
+      <c r="F11">
         <v>3</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>45</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>38</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -830,23 +853,24 @@
       <c r="D12" s="1">
         <v>388342.70040999999</v>
       </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
+      <c r="E12" s="10"/>
       <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12">
         <v>100</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1000</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -856,621 +880,744 @@
       <c r="D13" s="1">
         <v>408360.78125</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="10"/>
+      <c r="F13">
         <v>6</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>3508</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>102</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1">
+        <v>409850.32744999998</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1">
+        <v>421561.89714999998</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="J17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="K17" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C18" s="2">
         <v>0</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D18" s="1">
         <v>737883.09851000004</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E18" s="10"/>
+      <c r="F18" s="4">
+        <v>12</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>844281.16085975396</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>16537</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="J19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>849369.78633000003</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>424</v>
+      </c>
+      <c r="H20">
+        <v>300</v>
+      </c>
+      <c r="J20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>828745.59915999998</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>863676.299315896</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>940</v>
+      </c>
+      <c r="H22">
+        <v>1122</v>
+      </c>
+      <c r="J22" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>820394.24028599996</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23">
         <v>11</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="G23">
+        <v>30072</v>
+      </c>
+      <c r="H23">
+        <v>1000</v>
+      </c>
+      <c r="J23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1">
+        <v>776000.14246</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1">
+        <v>777475.78272599995</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26" s="1">
+        <v>846357.81419732003</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>77</v>
+      </c>
+      <c r="H26">
+        <v>72</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1">
+        <v>813544.21048000001</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1">
+        <v>851631.93099999998</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>9750</v>
+      </c>
+      <c r="H28">
+        <v>132</v>
+      </c>
+      <c r="J28" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1">
+        <v>846255.15026999998</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1">
+        <v>882383.30403208698</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1294974.2977</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="4">
+        <v>12</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C17">
+      <c r="C34">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
-        <v>844281.16085975396</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <v>16537</v>
-      </c>
-      <c r="G17">
+      <c r="D34" s="1">
+        <v>1476689.6626809801</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>17513</v>
+      </c>
+      <c r="H34">
         <v>50</v>
       </c>
-      <c r="I17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1">
-        <v>849369.78633000003</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="F18">
-        <v>424</v>
-      </c>
-      <c r="G18">
-        <v>300</v>
-      </c>
-      <c r="I18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1">
-        <v>828745.59915999998</v>
-      </c>
-      <c r="E19">
-        <v>6</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1">
-        <v>863676.299315896</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>940</v>
-      </c>
-      <c r="G20">
-        <v>1122</v>
-      </c>
-      <c r="I20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1">
-        <v>820394.24028599996</v>
-      </c>
-      <c r="E21">
-        <v>7</v>
-      </c>
-      <c r="F21">
-        <v>30072</v>
-      </c>
-      <c r="G21">
-        <v>1000</v>
-      </c>
-      <c r="I21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1">
-        <v>776000.14246</v>
-      </c>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1">
-        <v>777475.78272599995</v>
-      </c>
-      <c r="E23">
-        <v>9</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>8</v>
-      </c>
-      <c r="D24" s="1">
-        <v>846357.81419732003</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="F24">
-        <v>77</v>
-      </c>
-      <c r="G24">
-        <v>72</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25" s="1">
-        <v>813544.21048000001</v>
-      </c>
-      <c r="E25">
-        <v>8</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26" s="1">
-        <v>851631.93099999998</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26">
-        <v>9750</v>
-      </c>
-      <c r="G26">
-        <v>132</v>
-      </c>
-      <c r="I26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="2">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1294974.2977</v>
-      </c>
-      <c r="E29" s="4">
-        <v>11</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1476689.6626809801</v>
-      </c>
-      <c r="E30">
-        <v>4</v>
-      </c>
-      <c r="F30">
-        <v>17513</v>
-      </c>
-      <c r="G30">
-        <v>50</v>
-      </c>
-      <c r="H30">
+      <c r="I34">
         <f>4*3600</f>
         <v>14400</v>
       </c>
-      <c r="I30">
+      <c r="J34">
         <f>((4*60*60)/50)</f>
         <v>288</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>2</v>
       </c>
-      <c r="C31">
+      <c r="C35">
         <v>2</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D35" s="1">
         <v>1506388.4151300001</v>
       </c>
-      <c r="E31">
+      <c r="E35" s="10"/>
+      <c r="F35">
         <v>2</v>
       </c>
-      <c r="F31">
+      <c r="G35">
         <v>1000</v>
       </c>
-      <c r="G31">
+      <c r="H35">
         <v>1000</v>
       </c>
-      <c r="H31" s="9">
+      <c r="I35" s="9">
         <f>12*3600</f>
         <v>43200</v>
       </c>
-      <c r="I31">
+      <c r="J35">
         <f>(12*60*60)/1000</f>
         <v>43.2</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C32">
+      <c r="C36">
         <v>3</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D36" s="1">
         <v>1455075.6084199999</v>
       </c>
-      <c r="E32">
+      <c r="E36" s="10"/>
+      <c r="F36">
+        <v>11</v>
+      </c>
+      <c r="I36">
+        <v>15</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1513311.19361463</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <v>2988</v>
+      </c>
+      <c r="H37">
+        <v>2492</v>
+      </c>
+      <c r="I37">
+        <v>5299.01</v>
+      </c>
+      <c r="J37">
+        <v>5299.01</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>5</v>
       </c>
-      <c r="H32">
-        <v>15</v>
-      </c>
-      <c r="I32">
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1336164.5497999999</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38">
         <v>1</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1513311.19361463</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>2988</v>
-      </c>
-      <c r="G33">
-        <v>2492</v>
-      </c>
-      <c r="H33">
-        <v>5299.01</v>
-      </c>
-      <c r="I33">
-        <v>5299.01</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
-      </c>
-      <c r="D34" s="8">
-        <v>1336164.5497999999</v>
-      </c>
-      <c r="E34">
-        <v>9</v>
-      </c>
-      <c r="F34">
+      <c r="G38">
         <v>30113</v>
       </c>
-      <c r="G34">
+      <c r="H38">
         <v>500</v>
       </c>
-      <c r="H34">
+      <c r="I38">
         <f>8*3600</f>
         <v>28800</v>
       </c>
-      <c r="I34">
+      <c r="J38">
         <f>(8*60*60)/500</f>
         <v>57.6</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>6</v>
       </c>
-      <c r="C35">
+      <c r="C39">
         <v>6</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D39" s="1">
         <v>1364943.00774</v>
       </c>
-      <c r="E35">
+      <c r="E39" s="10"/>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>6000</v>
+      </c>
+      <c r="H39">
+        <v>300</v>
+      </c>
+      <c r="I39">
+        <v>318</v>
+      </c>
+      <c r="J39">
+        <v>318</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1332883.4328399999</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40">
         <v>8</v>
       </c>
-      <c r="F35">
-        <v>6000</v>
-      </c>
-      <c r="G35">
-        <v>300</v>
-      </c>
-      <c r="H35">
-        <v>318</v>
-      </c>
-      <c r="I35">
-        <v>318</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36">
-        <v>7</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1332883.4328399999</v>
-      </c>
-      <c r="E36">
-        <v>10</v>
-      </c>
-      <c r="H36">
+      <c r="I40">
         <f>(8*3600)+(46*60)</f>
         <v>31560</v>
       </c>
-      <c r="I36">
+      <c r="J40">
         <f>((8*60*60)+(46*60))/25</f>
         <v>1262.4000000000001</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>8</v>
       </c>
-      <c r="C37">
+      <c r="C41">
         <v>8</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D41" s="1">
         <v>1445967.377229</v>
       </c>
-      <c r="E37">
-        <v>6</v>
-      </c>
-      <c r="F37">
+      <c r="E41" s="10"/>
+      <c r="F41">
+        <v>9</v>
+      </c>
+      <c r="G41">
         <v>600</v>
       </c>
-      <c r="G37">
+      <c r="H41">
         <v>166</v>
       </c>
-      <c r="H37">
+      <c r="I41">
         <f>100*60</f>
         <v>6000</v>
       </c>
-      <c r="I37">
+      <c r="J41">
         <v>90</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>10</v>
       </c>
-      <c r="C38">
+      <c r="C42">
         <v>9</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D42" s="1">
         <v>1422268.7144299999</v>
       </c>
-      <c r="E38">
-        <v>7</v>
-      </c>
-      <c r="H38">
+      <c r="E42" s="10"/>
+      <c r="F42">
+        <v>6</v>
+      </c>
+      <c r="I42">
         <f>15*5</f>
         <v>75</v>
       </c>
-      <c r="I38">
+      <c r="J42">
         <v>5</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>11</v>
       </c>
-      <c r="C39">
+      <c r="C43">
         <v>10</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D43" s="1">
         <v>1480850.9759</v>
       </c>
-      <c r="E39">
-        <v>3</v>
-      </c>
-      <c r="F39">
+      <c r="E43" s="10"/>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
         <v>31979</v>
       </c>
-      <c r="G39">
+      <c r="H43">
         <v>246</v>
       </c>
-      <c r="H39">
+      <c r="I43">
         <v>193</v>
       </c>
-      <c r="I39">
+      <c r="J43">
         <v>193</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1484287.2607100001</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>12</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1526474.8024800699</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="F45">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>